<commit_message>
Atualizando Planilha de Horas
</commit_message>
<xml_diff>
--- a/Minha Planilha de Horas2.xlsx
+++ b/Minha Planilha de Horas2.xlsx
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="55">
   <si>
     <t xml:space="preserve">GERALDO LUIZ</t>
   </si>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">SRS</t>
   </si>
   <si>
-    <t xml:space="preserve">A compensar</t>
+    <t xml:space="preserve">Ausência por motivo de saúde</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,6 +789,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -823,12 +827,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -904,7 +908,7 @@
       <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -917,7 +921,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,7 +1880,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -1891,7 +1894,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3031,12 +3033,12 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -3051,7 +3053,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="56.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="1.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3067,7 +3068,7 @@
       </c>
       <c r="F1" s="3" t="n">
         <f aca="false">IF(E1="Compensou!!!",(J2-I2),IF((E1="Devendo:"),(I2-J2),"Deu erro"))</f>
-        <v>0.493749999999998</v>
+        <v>0.49375</v>
       </c>
       <c r="G1" s="4" t="n">
         <v>0.208333333333333</v>
@@ -3138,7 +3139,7 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="n">
         <f aca="false">IF(OR((B3=""),(C3="")),"",C3-B3)</f>
-        <v>0.176331018518518</v>
+        <v>0.176331018518519</v>
       </c>
       <c r="B3" s="14" t="n">
         <f aca="false">IF(SUM(B4:B34)&lt;=0,"",AVERAGE(B4:B34))</f>
@@ -3766,17 +3767,15 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
-      <c r="K20" s="27" t="s">
-        <v>54</v>
-      </c>
+      <c r="K20" s="27"/>
       <c r="L20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="n">
         <v>43908</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="21"/>
       <c r="E21" s="22" t="str">
         <f aca="false">IF(AND(B21&gt;1,B21&gt;1),"",IF(OR(B21&gt;1,C21&gt;1),"",IF(C21&gt;B21,C21-B21,"")))</f>
@@ -3796,7 +3795,9 @@
       </c>
       <c r="I21" s="26"/>
       <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
+      <c r="K21" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,7 +3825,9 @@
       </c>
       <c r="I22" s="26"/>
       <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
+      <c r="K22" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L22" s="50"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,7 +3855,9 @@
       </c>
       <c r="I23" s="26"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
+      <c r="K23" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L23" s="50"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3936,7 +3941,9 @@
       </c>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
+      <c r="K26" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,7 +3971,9 @@
       </c>
       <c r="I27" s="26"/>
       <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
+      <c r="K27" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +4001,9 @@
       </c>
       <c r="I28" s="26"/>
       <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
+      <c r="K28" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4020,7 +4031,9 @@
       </c>
       <c r="I29" s="26"/>
       <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
+      <c r="K29" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L29" s="50"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4048,7 +4061,9 @@
       </c>
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
+      <c r="K30" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L30" s="50"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4132,7 +4147,9 @@
       </c>
       <c r="I33" s="26"/>
       <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
+      <c r="K33" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4160,7 +4177,9 @@
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="K34" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="L34" s="50"/>
     </row>
   </sheetData>
@@ -4192,7 +4211,7 @@
       <selection pane="bottomLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -4206,7 +4225,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5318,59 +5336,57 @@
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="53"/>
+      <c r="A1" s="54"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="n">
+      <c r="A2" s="55" t="n">
         <v>220000</v>
       </c>
-      <c r="B2" s="55" t="n">
+      <c r="B2" s="56" t="n">
         <v>0.04</v>
       </c>
-      <c r="C2" s="54" t="n">
+      <c r="C2" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)</f>
         <v>228800</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57" t="n">
+      <c r="D2" s="57"/>
+      <c r="E2" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C26</f>
         <v>5720000</v>
       </c>
-      <c r="G2" s="56" t="n">
+      <c r="G2" s="57" t="n">
         <v>220000</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I2" s="56" t="n">
+      <c r="I2" s="57" t="n">
         <f aca="false">H2*G2</f>
         <v>2640000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="54" t="n">
+      <c r="A3" s="55"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C2</f>
         <v>457600</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57" t="n">
+      <c r="D3" s="57"/>
+      <c r="E3" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E2</f>
         <v>5948800</v>
       </c>
@@ -5383,279 +5399,279 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="54" t="n">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C3</f>
         <v>686400</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="57" t="n">
+      <c r="D4" s="57"/>
+      <c r="E4" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E3</f>
         <v>6177600</v>
       </c>
-      <c r="I4" s="56" t="n">
+      <c r="I4" s="57" t="n">
         <f aca="false">(I2*I3)/12+I2</f>
         <v>2745600</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="54" t="n">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C4</f>
         <v>915200</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="57" t="n">
+      <c r="D5" s="57"/>
+      <c r="E5" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E4</f>
         <v>6406400</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="54" t="n">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C5</f>
         <v>1144000</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57" t="n">
+      <c r="D6" s="57"/>
+      <c r="E6" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E5</f>
         <v>6635200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="54" t="n">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C6</f>
         <v>1372800</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57" t="n">
+      <c r="D7" s="57"/>
+      <c r="E7" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E6</f>
         <v>6864000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="54" t="n">
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C7</f>
         <v>1601600</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57" t="n">
+      <c r="D8" s="57"/>
+      <c r="E8" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E7</f>
         <v>7092800</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="54" t="n">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C8</f>
         <v>1830400</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57" t="n">
+      <c r="D9" s="57"/>
+      <c r="E9" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E8</f>
         <v>7321600</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="54" t="n">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C9</f>
         <v>2059200</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57" t="n">
+      <c r="D10" s="57"/>
+      <c r="E10" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E9</f>
         <v>7550400</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="54"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="54" t="n">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C10</f>
         <v>2288000</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57" t="n">
+      <c r="D11" s="57"/>
+      <c r="E11" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E10</f>
         <v>7779200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="54"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="54" t="n">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C11</f>
         <v>2516800</v>
       </c>
-      <c r="D12" s="56"/>
-      <c r="E12" s="57" t="n">
+      <c r="D12" s="57"/>
+      <c r="E12" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E11</f>
         <v>8008000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="54"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="54" t="n">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="55" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C12</f>
         <v>2745600</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57" t="n">
+      <c r="D13" s="57"/>
+      <c r="E13" s="58" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E12</f>
         <v>8236800</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="58" t="n">
+      <c r="A15" s="59"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C13</f>
         <v>2974400</v>
       </c>
-      <c r="E15" s="60" t="n">
+      <c r="E15" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E13</f>
         <v>8465600</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="58" t="n">
+      <c r="A16" s="59"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C15</f>
         <v>3203200</v>
       </c>
-      <c r="E16" s="60" t="n">
+      <c r="E16" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E15</f>
         <v>8694400</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="58" t="n">
+      <c r="A17" s="59"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C16</f>
         <v>3432000</v>
       </c>
-      <c r="E17" s="60" t="n">
+      <c r="E17" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E16</f>
         <v>8923200</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="58" t="n">
+      <c r="A18" s="59"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C17</f>
         <v>3660800</v>
       </c>
-      <c r="E18" s="60" t="n">
+      <c r="E18" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E17</f>
         <v>9152000</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="58" t="n">
+      <c r="A19" s="59"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C18</f>
         <v>3889600</v>
       </c>
-      <c r="E19" s="60" t="n">
+      <c r="E19" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E18</f>
         <v>9380800</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="58" t="n">
+      <c r="A20" s="59"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C19</f>
         <v>4118400</v>
       </c>
-      <c r="E20" s="60" t="n">
+      <c r="E20" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E19</f>
         <v>9609600</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="58" t="n">
+      <c r="A21" s="59"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C20</f>
         <v>4347200</v>
       </c>
-      <c r="E21" s="60" t="n">
+      <c r="E21" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E20</f>
         <v>9838400</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="58"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="58" t="n">
+      <c r="A22" s="59"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C21</f>
         <v>4576000</v>
       </c>
-      <c r="E22" s="60" t="n">
+      <c r="E22" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E21</f>
         <v>10067200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="58"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="58" t="n">
+      <c r="A23" s="59"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C22</f>
         <v>4804800</v>
       </c>
-      <c r="E23" s="60" t="n">
+      <c r="E23" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E22</f>
         <v>10296000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="58" t="n">
+      <c r="A24" s="59"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C23</f>
         <v>5033600</v>
       </c>
-      <c r="E24" s="60" t="n">
+      <c r="E24" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E23</f>
         <v>10524800</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="58" t="n">
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C24</f>
         <v>5262400</v>
       </c>
-      <c r="E25" s="60" t="n">
+      <c r="E25" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E24</f>
         <v>10753600</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="58" t="n">
+      <c r="A26" s="59"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="59" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+C25</f>
         <v>5491200</v>
       </c>
-      <c r="E26" s="60" t="n">
+      <c r="E26" s="61" t="n">
         <f aca="false">$A$2+($A$2*$B$2)+E25</f>
         <v>10982400</v>
       </c>
@@ -5682,7 +5698,7 @@
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -5696,7 +5712,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6810,7 +6825,7 @@
       <selection pane="bottomLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -6823,7 +6838,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,7 +7915,7 @@
       <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -7915,7 +7929,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9047,7 +9060,7 @@
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -9061,8 +9074,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="34" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="34" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10194,7 +10206,7 @@
       <selection pane="bottomLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -10208,7 +10220,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11338,7 +11349,7 @@
       <selection pane="bottomLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -11352,7 +11363,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12499,7 +12509,7 @@
       <selection pane="bottomLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -12513,7 +12523,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13665,7 +13674,7 @@
       <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -13679,7 +13688,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14835,7 +14843,7 @@
       <selection pane="bottomLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -14849,7 +14857,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>